<commit_message>
Agregué información sobre la hoja de balance de alimentos
</commit_message>
<xml_diff>
--- a/docs/cuadrosfiguraSAN.xlsx
+++ b/docs/cuadrosfiguraSAN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="0" windowWidth="17660" windowHeight="18000" tabRatio="978" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="11140" yWindow="0" windowWidth="17660" windowHeight="18000" tabRatio="978" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Oferta Prods Agrícolas" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Oferta monetaria" sheetId="9" r:id="rId9"/>
     <sheet name="Utilización Monetaria" sheetId="10" r:id="rId10"/>
     <sheet name="Cuentas de producción e ingreso" sheetId="11" r:id="rId11"/>
+    <sheet name="Consumo fertilizantes" sheetId="12" r:id="rId12"/>
+    <sheet name="Calorías per cápita" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="191">
   <si>
     <t>Cuadro 1</t>
   </si>
@@ -593,16 +595,68 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Consumo de fertilizantes (kilogramos por hectárea de tierras cultivables)</t>
+  </si>
+  <si>
+    <t>Fertilizantes y nutrientes</t>
+  </si>
+  <si>
+    <t>Consumo de fertilizantes</t>
+  </si>
+  <si>
+    <t>Años 2002-2013</t>
+  </si>
+  <si>
+    <t>(kg/ha de tierras cultivables)</t>
+  </si>
+  <si>
+    <t>Fuente: FAO (2016).</t>
+  </si>
+  <si>
+    <t>Caloría vegetal</t>
+  </si>
+  <si>
+    <t>Caloría animal</t>
+  </si>
+  <si>
+    <t>Caloría total</t>
+  </si>
+  <si>
+    <t>Disponibilidad de calorías totales</t>
+  </si>
+  <si>
+    <t>Años 2005-2013</t>
+  </si>
+  <si>
+    <t>(calorías per cápita diarias)</t>
+  </si>
+  <si>
+    <t>Fuente: Ine (2013)</t>
+  </si>
+  <si>
+    <t>Figura 3</t>
+  </si>
+  <si>
+    <t>Datos  figura</t>
+  </si>
+  <si>
+    <t>Porcentajes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -649,6 +703,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -658,7 +719,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -677,12 +738,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -721,8 +792,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -734,6 +823,1117 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calorías per cápita'!$B$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Caloría vegetal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Calorías per cápita'!$A$30:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calorías per cápita'!$B$30:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1757.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2182.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2144.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2391.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2909.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2792.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2796.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2676.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2423.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calorías per cápita'!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Caloría animal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Calorías per cápita'!$A$30:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calorías per cápita'!$C$30:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>491.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>411.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>418.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>349.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>314.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>425.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>293.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>232.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2078781136"/>
+        <c:axId val="-2073121136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2078781136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2073121136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2073121136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2078781136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2481,10 +3681,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK13"/>
+  <dimension ref="A1:AMK21"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2701,6 +3901,55 @@
         <v>676754.25739278505</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2709,43 +3958,42 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="53" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>154</v>
@@ -2766,7 +4014,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>135</v>
       </c>
@@ -2789,8 +4037,24 @@
         <f t="shared" ref="G7:G20" si="0">F7/F$20*100</f>
         <v>1.5110683172813986</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I7" s="7">
+        <f t="shared" ref="I7:K20" si="1">B7/B$20*100</f>
+        <v>0.15715929392153821</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.92151912024157745</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="1"/>
+        <v>3.3526447246895672</v>
+      </c>
+      <c r="L7" s="7">
+        <f>E7/E$20*100</f>
+        <v>1.005750721809799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>136</v>
       </c>
@@ -2813,8 +4077,24 @@
         <f t="shared" si="0"/>
         <v>0.87794492124045109</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11635589325767497</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>1.6691981098449387</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="1"/>
+        <v>2.376739486033046E-2</v>
+      </c>
+      <c r="L8" s="7">
+        <f>E8/E$20*100</f>
+        <v>0.44073124118970219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>137</v>
       </c>
@@ -2837,8 +4117,24 @@
         <f t="shared" si="0"/>
         <v>0.61958943535242694</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.27224170649796903</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.45130396497574604</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5365710742309813</v>
+      </c>
+      <c r="L9" s="7">
+        <f>E9/E$20*100</f>
+        <v>0.19211491799784128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>138</v>
       </c>
@@ -2861,8 +4157,24 @@
         <f t="shared" si="0"/>
         <v>0.89670652870978318</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.0886517683435686</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.1372861209660802</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>2.8769482212744544</v>
+      </c>
+      <c r="L10" s="7">
+        <f>E10/E$20*100</f>
+        <v>0.4896229131012792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>139</v>
       </c>
@@ -2885,8 +4197,24 @@
         <f t="shared" si="0"/>
         <v>2.4786657716824321</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.22415860933099382</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.29105739792473889</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="1"/>
+        <v>8.9195290334954187</v>
+      </c>
+      <c r="L11" s="7">
+        <f>E11/E$20*100</f>
+        <v>0.83106501552093148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>140</v>
       </c>
@@ -2909,8 +4237,24 @@
         <f t="shared" si="0"/>
         <v>1.1062751816437142</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.2754379221730916</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1646797533969517</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1243019272530637</v>
+      </c>
+      <c r="L12" s="7">
+        <f>E12/E$20*100</f>
+        <v>0.30932772611482873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>141</v>
       </c>
@@ -2933,8 +4277,24 @@
         <f t="shared" si="0"/>
         <v>0.98184829580843425</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.65948632504429128</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>1.266640644830703</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.88773668967818808</v>
+      </c>
+      <c r="L13" s="7">
+        <f>E13/E$20*100</f>
+        <v>0.67147866724478833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>142</v>
       </c>
@@ -2957,8 +4317,24 @@
         <f t="shared" si="0"/>
         <v>2.3189643714846109</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.13293556629552944</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>1.8520382265337583</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="1"/>
+        <v>4.8022051989899106</v>
+      </c>
+      <c r="L14" s="7">
+        <f>E14/E$20*100</f>
+        <v>1.2016098716606602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>143</v>
       </c>
@@ -2981,8 +4357,24 @@
         <f t="shared" si="0"/>
         <v>0.64180398539834393</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I15" s="7">
+        <f t="shared" si="1"/>
+        <v>0.44272224631252161</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>0.16768816515306056</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="1"/>
+        <v>2.016961409272406</v>
+      </c>
+      <c r="L15" s="7">
+        <f>E15/E$20*100</f>
+        <v>0.29386087222935864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>144</v>
       </c>
@@ -3005,8 +4397,24 @@
         <f t="shared" si="0"/>
         <v>0.20455299171222541</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.30555326693475304</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32387839919282424</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.1557894725845046</v>
+      </c>
+      <c r="L16" s="7">
+        <f>E16/E$20*100</f>
+        <v>7.6481080857155867E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>145</v>
       </c>
@@ -3029,8 +4437,24 @@
         <f t="shared" si="0"/>
         <v>26.687341787773729</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I17" s="7">
+        <f t="shared" si="1"/>
+        <v>29.472315974262415</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>24.606392866514799</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="1"/>
+        <v>28.682427446877725</v>
+      </c>
+      <c r="L17" s="7">
+        <f>E17/E$20*100</f>
+        <v>28.002824139395639</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>146</v>
       </c>
@@ -3053,8 +4477,24 @@
         <f t="shared" si="0"/>
         <v>2.1575323753218703</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I18" s="7">
+        <f t="shared" si="1"/>
+        <v>1.4968084609823209</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="1"/>
+        <v>3.8627539499941759</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="1"/>
+        <v>1.6088725508608373E-4</v>
+      </c>
+      <c r="L18" s="7">
+        <f>E18/E$20*100</f>
+        <v>1.42398137263791</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>147</v>
       </c>
@@ -3077,8 +4517,24 @@
         <f t="shared" si="0"/>
         <v>59.517706036590525</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I19" s="7">
+        <f t="shared" si="1"/>
+        <v>65.356172966643427</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>63.285563280430637</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="1"/>
+        <v>44.62095651953836</v>
+      </c>
+      <c r="L19" s="7">
+        <f>E19/E$20*100</f>
+        <v>65.061151460240112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -3101,10 +4557,486 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="I20" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="L20" s="7">
+        <f>E20/E$20*100</f>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="30"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="30"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="30"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="30"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="30"/>
+    </row>
+    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:2" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="26">
+        <v>2002</v>
+      </c>
+      <c r="B8" s="11">
+        <v>99.790175438596492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="26">
+        <v>2003</v>
+      </c>
+      <c r="B9" s="11">
+        <v>91.671826625386998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="26">
+        <v>2004</v>
+      </c>
+      <c r="B10" s="11">
+        <v>124.94625000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="26">
+        <v>2005</v>
+      </c>
+      <c r="B11" s="11">
+        <v>141.69071428571428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="26">
+        <v>2006</v>
+      </c>
+      <c r="B12" s="11">
+        <v>136.04382470119521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="26">
+        <v>2007</v>
+      </c>
+      <c r="B13" s="11">
+        <v>123.7734771573604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="26">
+        <v>2008</v>
+      </c>
+      <c r="B14" s="11">
+        <v>92.005283018867928</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="26">
+        <v>2009</v>
+      </c>
+      <c r="B15" s="11">
+        <v>127.06855791962175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="26">
+        <v>2010</v>
+      </c>
+      <c r="B16" s="11">
+        <v>189.14955521369808</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="26">
+        <v>2011</v>
+      </c>
+      <c r="B17" s="11">
+        <v>223.1941817924745</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="26">
+        <v>2012</v>
+      </c>
+      <c r="B18" s="11">
+        <v>250.16492372277821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>2013</v>
+      </c>
+      <c r="B19" s="28">
+        <v>255.49017652338685</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F28" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="32">
+        <v>2005</v>
+      </c>
+      <c r="B30" s="32">
+        <v>1757</v>
+      </c>
+      <c r="C30" s="32">
+        <v>491</v>
+      </c>
+      <c r="D30" s="32">
+        <f>SUM(B30:C30)</f>
+        <v>2248</v>
+      </c>
+      <c r="F30" s="32">
+        <v>2005</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="32">
+        <v>2006</v>
+      </c>
+      <c r="B31" s="32">
+        <v>2182</v>
+      </c>
+      <c r="C31" s="32">
+        <v>411</v>
+      </c>
+      <c r="D31" s="32">
+        <f t="shared" ref="D31:D38" si="0">SUM(B31:C31)</f>
+        <v>2593</v>
+      </c>
+      <c r="F31" s="32">
+        <v>2006</v>
+      </c>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="32">
+        <v>2007</v>
+      </c>
+      <c r="B32" s="32">
+        <v>2144</v>
+      </c>
+      <c r="C32" s="32">
+        <v>418</v>
+      </c>
+      <c r="D32" s="32">
+        <f t="shared" si="0"/>
+        <v>2562</v>
+      </c>
+      <c r="F32" s="32">
+        <v>2007</v>
+      </c>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="32">
+        <v>2008</v>
+      </c>
+      <c r="B33" s="32">
+        <v>2391</v>
+      </c>
+      <c r="C33" s="32">
+        <v>349</v>
+      </c>
+      <c r="D33" s="32">
+        <f t="shared" si="0"/>
+        <v>2740</v>
+      </c>
+      <c r="F33" s="32">
+        <v>2008</v>
+      </c>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="32">
+        <v>2009</v>
+      </c>
+      <c r="B34" s="32">
+        <v>2909</v>
+      </c>
+      <c r="C34" s="32">
+        <v>314</v>
+      </c>
+      <c r="D34" s="32">
+        <f t="shared" si="0"/>
+        <v>3223</v>
+      </c>
+      <c r="F34" s="32">
+        <v>2009</v>
+      </c>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="32">
+        <v>2010</v>
+      </c>
+      <c r="B35" s="32">
+        <v>2792</v>
+      </c>
+      <c r="C35" s="32">
+        <v>425</v>
+      </c>
+      <c r="D35" s="32">
+        <f t="shared" si="0"/>
+        <v>3217</v>
+      </c>
+      <c r="F35" s="32">
+        <v>2010</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="32">
+        <v>2011</v>
+      </c>
+      <c r="B36" s="32">
+        <v>2796</v>
+      </c>
+      <c r="C36" s="32">
+        <v>293</v>
+      </c>
+      <c r="D36" s="32">
+        <f t="shared" si="0"/>
+        <v>3089</v>
+      </c>
+      <c r="F36" s="32">
+        <v>2011</v>
+      </c>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="32">
+        <v>2012</v>
+      </c>
+      <c r="B37" s="32">
+        <v>2676</v>
+      </c>
+      <c r="C37" s="32">
+        <v>420</v>
+      </c>
+      <c r="D37" s="32">
+        <f t="shared" si="0"/>
+        <v>3096</v>
+      </c>
+      <c r="F37" s="32">
+        <v>2012</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="32">
+        <v>2013</v>
+      </c>
+      <c r="B38" s="32">
+        <v>2423</v>
+      </c>
+      <c r="C38" s="32">
+        <v>232</v>
+      </c>
+      <c r="D38" s="32">
+        <f t="shared" si="0"/>
+        <v>2655</v>
+      </c>
+      <c r="F38" s="32">
+        <v>2013</v>
+      </c>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D30:D38" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9018,10 +10950,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9030,7 +10962,7 @@
     <col min="2" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>95</v>
       </c>
@@ -9043,7 +10975,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>96</v>
       </c>
@@ -9056,7 +10988,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>97</v>
       </c>
@@ -9069,7 +11001,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
@@ -9082,7 +11014,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>98</v>
       </c>
@@ -9095,7 +11027,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="4" t="s">
         <v>99</v>
@@ -9122,7 +11054,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -9150,8 +11082,9 @@
       <c r="I7" s="9">
         <v>2569739259.9149199</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -9179,8 +11112,9 @@
       <c r="I8" s="9">
         <v>1433998152.56497</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -9208,8 +11142,9 @@
       <c r="I9" s="9">
         <v>670418977.89874303</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -9237,8 +11172,9 @@
       <c r="I10" s="9">
         <v>56178995.368562199</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -9266,8 +11202,9 @@
       <c r="I11" s="9">
         <v>4819393423.9791002</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -9295,8 +11232,9 @@
       <c r="I12" s="9">
         <v>156494783.120231</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -9324,8 +11262,9 @@
       <c r="I13" s="9">
         <v>2672319.4391717501</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>106</v>
       </c>
@@ -9353,8 +11292,9 @@
       <c r="I14" s="9">
         <v>817281.99388686195</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
@@ -9382,8 +11322,9 @@
       <c r="I15" s="9">
         <v>124480070.612846</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
@@ -9411,8 +11352,9 @@
       <c r="I16" s="9">
         <v>12695274.525811501</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
@@ -9440,8 +11382,9 @@
       <c r="I17" s="9">
         <v>130905998.17559899</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>27</v>
       </c>
@@ -9469,8 +11412,9 @@
       <c r="I18" s="9">
         <v>278816582.23354203</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
@@ -9498,8 +11442,9 @@
       <c r="I19" s="9">
         <v>3619141.1316</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -9527,8 +11472,9 @@
       <c r="I20" s="9">
         <v>91845671.0466232</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>107</v>
       </c>
@@ -9556,8 +11502,9 @@
       <c r="I21" s="9">
         <v>200943973.448513</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>108</v>
       </c>
@@ -9585,8 +11532,9 @@
       <c r="I22" s="9">
         <v>80351449.4001517</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>109</v>
       </c>
@@ -9614,8 +11562,9 @@
       <c r="I23" s="9">
         <v>161272669.18539</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>110</v>
       </c>
@@ -9643,8 +11592,9 @@
       <c r="I24" s="9">
         <v>428134559.79486799</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>111</v>
       </c>
@@ -9672,8 +11622,9 @@
       <c r="I25" s="9">
         <v>90363654.795937702</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>112</v>
       </c>
@@ -9701,8 +11652,9 @@
       <c r="I26" s="9">
         <v>2875173808.06599</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
@@ -9730,8 +11682,9 @@
       <c r="I27" s="9">
         <v>28093581.304467399</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
@@ -9759,8 +11712,9 @@
       <c r="I28" s="9">
         <v>17699413.399346899</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
@@ -9788,8 +11742,9 @@
       <c r="I29" s="9">
         <v>18492579.855480701</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
@@ -9817,8 +11772,9 @@
       <c r="I30" s="9">
         <v>931612203.55445004</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -9846,8 +11802,9 @@
       <c r="I31" s="9">
         <v>640766.37104970496</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>113</v>
       </c>
@@ -9875,8 +11832,9 @@
       <c r="I32" s="9">
         <v>193103918.05677199</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>114</v>
       </c>
@@ -9904,8 +11862,9 @@
       <c r="I33" s="9">
         <v>2264092.6783230002</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>19</v>
       </c>
@@ -9933,8 +11892,9 @@
       <c r="I34" s="9">
         <v>35607815.451540202</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>23</v>
       </c>
@@ -9962,8 +11922,9 @@
       <c r="I35" s="9">
         <v>51347892.767319001</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
@@ -9991,8 +11952,9 @@
       <c r="I36" s="9">
         <v>17117279.240500301</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>116</v>
       </c>
@@ -10020,8 +11982,9 @@
       <c r="I37" s="9">
         <v>74526649.596314698</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>117</v>
       </c>
@@ -10049,8 +12012,9 @@
       <c r="I38" s="9">
         <v>534375923.81106102</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
@@ -10078,8 +12042,9 @@
       <c r="I39" s="9">
         <v>42752778.796714097</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>43</v>
       </c>
@@ -10107,8 +12072,9 @@
       <c r="I40" s="9">
         <v>4811514151.04743</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>41</v>
       </c>
@@ -10136,8 +12102,9 @@
       <c r="I41" s="9">
         <v>135900.24138198001</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>118</v>
       </c>
@@ -10165,8 +12132,9 @@
       <c r="I42" s="9">
         <v>135461841.74758801</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>119</v>
       </c>
@@ -10194,8 +12162,9 @@
       <c r="I43" s="9">
         <v>12342437.3380189</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
@@ -10223,8 +12192,9 @@
       <c r="I44" s="9">
         <v>6168010.4674088201</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>38</v>
       </c>
@@ -10252,8 +12222,9 @@
       <c r="I45" s="9">
         <v>15498414.9428245</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>120</v>
       </c>
@@ -10281,8 +12252,9 @@
       <c r="I46" s="9">
         <v>25693117.569694601</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>8</v>
       </c>
@@ -10319,9 +12291,39 @@
         <v>21142764814.934147</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C51" s="7">
+        <f>C40/$I40*100</f>
+        <v>56.074627272226294</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" ref="D51:I51" si="1">D40/$I40*100</f>
+        <v>23.479991900091647</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" si="1"/>
+        <v>0.34864230395397711</v>
+      </c>
+      <c r="F51" s="7">
+        <f t="shared" si="1"/>
+        <v>16.734830591401366</v>
+      </c>
+      <c r="G51" s="7">
+        <f t="shared" si="1"/>
+        <v>3.3619079323268202</v>
+      </c>
+      <c r="H51" s="7">
+        <f t="shared" si="1"/>
+        <v>43.925372727773905</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -10339,10 +12341,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10351,32 +12353,32 @@
     <col min="2" max="13" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="66" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="4" t="s">
         <v>124</v>
@@ -10415,7 +12417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>135</v>
       </c>
@@ -10456,8 +12458,16 @@
         <f t="shared" ref="M7:M23" si="0">SUM(B7:L7)</f>
         <v>732.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="23">
+        <f>SUM(M7:M13)</f>
+        <v>3826.4</v>
+      </c>
+      <c r="O7" s="22">
+        <f>N7/N$23*100</f>
+        <v>0.73501544504412986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>136</v>
       </c>
@@ -10498,8 +12508,12 @@
         <f t="shared" si="0"/>
         <v>218.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="22">
+        <f t="shared" ref="O8:O23" si="1">N8/N$23*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>137</v>
       </c>
@@ -10540,8 +12554,12 @@
         <f t="shared" si="0"/>
         <v>115.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O9" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>138</v>
       </c>
@@ -10582,8 +12600,12 @@
         <f t="shared" si="0"/>
         <v>1230.0999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O10" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>139</v>
       </c>
@@ -10624,8 +12646,12 @@
         <f t="shared" si="0"/>
         <v>871.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O11" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>140</v>
       </c>
@@ -10666,8 +12692,12 @@
         <f t="shared" si="0"/>
         <v>439.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>141</v>
       </c>
@@ -10708,8 +12738,12 @@
         <f t="shared" si="0"/>
         <v>218.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>142</v>
       </c>
@@ -10750,8 +12784,16 @@
         <f t="shared" si="0"/>
         <v>1658.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="23">
+        <f>M14</f>
+        <v>1658.5</v>
+      </c>
+      <c r="O14" s="22">
+        <f t="shared" si="1"/>
+        <v>0.31858224848570177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>143</v>
       </c>
@@ -10792,8 +12834,16 @@
         <f t="shared" si="0"/>
         <v>1019.4000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="23">
+        <f t="shared" ref="N15:N23" si="2">M15</f>
+        <v>1019.4000000000001</v>
+      </c>
+      <c r="O15" s="22">
+        <f t="shared" si="1"/>
+        <v>0.19581715050125079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>144</v>
       </c>
@@ -10834,8 +12884,16 @@
         <f t="shared" si="0"/>
         <v>176.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="23">
+        <f t="shared" si="2"/>
+        <v>176.8</v>
+      </c>
+      <c r="O16" s="22">
+        <f t="shared" si="1"/>
+        <v>3.3961616841888503E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>145</v>
       </c>
@@ -10876,8 +12934,16 @@
         <f t="shared" si="0"/>
         <v>105114</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="23">
+        <f t="shared" si="2"/>
+        <v>105114</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" si="1"/>
+        <v>20.191410592297895</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>146</v>
       </c>
@@ -10918,8 +12984,16 @@
         <f t="shared" si="0"/>
         <v>74172.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="23">
+        <f t="shared" si="2"/>
+        <v>74172.5</v>
+      </c>
+      <c r="O18" s="22">
+        <f t="shared" si="1"/>
+        <v>14.247839509077911</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>147</v>
       </c>
@@ -10960,8 +13034,16 @@
         <f t="shared" si="0"/>
         <v>60077.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="23">
+        <f t="shared" si="2"/>
+        <v>60077.5</v>
+      </c>
+      <c r="O19" s="22">
+        <f t="shared" si="1"/>
+        <v>11.540322600783689</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
@@ -11002,8 +13084,16 @@
         <f t="shared" si="0"/>
         <v>247676.00000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="23">
+        <f t="shared" si="2"/>
+        <v>247676.00000000003</v>
+      </c>
+      <c r="O20" s="22">
+        <f t="shared" si="1"/>
+        <v>47.576229711151456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>56</v>
       </c>
@@ -11044,8 +13134,16 @@
         <f t="shared" si="0"/>
         <v>22129.399999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="23">
+        <f t="shared" si="2"/>
+        <v>22129.399999999998</v>
+      </c>
+      <c r="O21" s="22">
+        <f t="shared" si="1"/>
+        <v>4.2508495686701773</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>148</v>
       </c>
@@ -11086,58 +13184,88 @@
         <f t="shared" si="0"/>
         <v>4737.1999999999989</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="23">
+        <f t="shared" si="2"/>
+        <v>4737.1999999999989</v>
+      </c>
+      <c r="O22" s="22">
+        <f t="shared" si="1"/>
+        <v>0.90997155714589462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="8">
-        <f t="shared" ref="B23:L23" si="1">SUM(B7:B22)</f>
+        <f t="shared" ref="B23:L23" si="3">SUM(B7:B22)</f>
         <v>247381.8</v>
       </c>
       <c r="C23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25402.5</v>
       </c>
       <c r="D23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34178.5</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44416.499999999993</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52970.100000000006</v>
       </c>
       <c r="G23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>23802.500000000004</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3299.8999999999996</v>
       </c>
       <c r="I23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14559.8</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4123.8999999999996</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40980.199999999997</v>
       </c>
       <c r="L23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>29471.999999999996</v>
       </c>
       <c r="M23" s="8">
         <f t="shared" si="0"/>
         <v>520587.70000000007</v>
+      </c>
+      <c r="N23" s="23">
+        <f t="shared" si="2"/>
+        <v>520587.70000000007</v>
+      </c>
+      <c r="O23" s="22">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D27" s="7">
+        <f>B20/$M$23*100</f>
+        <v>39.968289684908029</v>
+      </c>
+      <c r="E27" s="7">
+        <f>I20/$M$23*100</f>
+        <v>1.3340883774242072</v>
+      </c>
+      <c r="F27" s="7">
+        <f>L20/$M$23*100</f>
+        <v>1.2772295618970635</v>
       </c>
     </row>
   </sheetData>
@@ -11150,8 +13278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11160,7 +13288,7 @@
     <col min="2" max="1025" width="8.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>149</v>
       </c>
@@ -11170,7 +13298,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>150</v>
       </c>
@@ -11180,7 +13308,7 @@
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>151</v>
       </c>
@@ -11190,7 +13318,7 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -11200,7 +13328,7 @@
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>152</v>
       </c>
@@ -11210,7 +13338,7 @@
       <c r="E5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>153</v>
@@ -11228,7 +13356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>156</v>
       </c>
@@ -11247,8 +13375,12 @@
       <c r="F7" s="17">
         <v>61145.121938784403</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="25">
+        <f>F7/F$13*100</f>
+        <v>9.0350533122512005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>157</v>
       </c>
@@ -11267,8 +13399,12 @@
       <c r="F8" s="17">
         <v>10507.1675182256</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="25">
+        <f t="shared" ref="G8:G13" si="0">F8/F$13*100</f>
+        <v>1.5525820487031601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>158</v>
       </c>
@@ -11287,8 +13423,12 @@
       <c r="F9" s="17">
         <v>4957.8112940324299</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="25">
+        <f t="shared" si="0"/>
+        <v>0.732586475148579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>159</v>
       </c>
@@ -11307,8 +13447,12 @@
       <c r="F10" s="17">
         <v>6400.7108355999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="25">
+        <f t="shared" si="0"/>
+        <v>0.94579521312995896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>160</v>
       </c>
@@ -11327,8 +13471,12 @@
       <c r="F11" s="17">
         <v>1474.23556453893</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="25">
+        <f t="shared" si="0"/>
+        <v>0.21783907690561358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>161</v>
       </c>
@@ -11347,8 +13495,12 @@
       <c r="F12" s="17">
         <v>592269.36508758098</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="25">
+        <f t="shared" si="0"/>
+        <v>87.516143873861537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
@@ -11366,6 +13518,10 @@
       </c>
       <c r="F13" s="18">
         <v>676754.41223876202</v>
+      </c>
+      <c r="G13" s="25">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>